<commit_message>
Jira'dan alınan verilerin sunumu için Excel'e yazdırma işlemi tamamlanmıştır.
</commit_message>
<xml_diff>
--- a/StajProje.xlsx
+++ b/StajProje.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilayd\Desktop\Staj Proje\Staj\StajProje\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilayd\Desktop\Staj Proje\Staj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{725CBE3C-88BC-41E5-817C-CE6C4A7C498D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A8E3005-BA1B-4210-88CC-39E7522FB2A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{E2AB668E-2BF8-4DD7-8D36-14A3C8896B93}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{31485E87-BFA0-45B0-A864-5FA1EB241FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -26,16 +26,115 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t>Transition ID</t>
+  </si>
+  <si>
+    <t>Number of Changed Status</t>
+  </si>
+  <si>
+    <t>TSI-28</t>
+  </si>
+  <si>
+    <t>TSI-27</t>
+  </si>
+  <si>
+    <t>TSI-26</t>
+  </si>
+  <si>
+    <t>TSI-25</t>
+  </si>
+  <si>
+    <t>TSI-24</t>
+  </si>
+  <si>
+    <t>TSI-23</t>
+  </si>
+  <si>
+    <t>TSI-22</t>
+  </si>
+  <si>
+    <t>TSI-21</t>
+  </si>
+  <si>
+    <t>TSI-20</t>
+  </si>
+  <si>
+    <t>TSI-19</t>
+  </si>
+  <si>
+    <t>TSI-16</t>
+  </si>
+  <si>
+    <t>TSI-15</t>
+  </si>
+  <si>
+    <t>TSI-14</t>
+  </si>
+  <si>
+    <t>TSI-13</t>
+  </si>
+  <si>
+    <t>TSI-12</t>
+  </si>
+  <si>
+    <t>TSI-11</t>
+  </si>
+  <si>
+    <t>TSI-10</t>
+  </si>
+  <si>
+    <t>TSI-9</t>
+  </si>
+  <si>
+    <t>TSI-8</t>
+  </si>
+  <si>
+    <t>TSI-7</t>
+  </si>
+  <si>
+    <t>TSI-6</t>
+  </si>
+  <si>
+    <t>TSI-5</t>
+  </si>
+  <si>
+    <t>TSI-4</t>
+  </si>
+  <si>
+    <t>TSI-3</t>
+  </si>
+  <si>
+    <t>TSI-2</t>
+  </si>
+  <si>
+    <t>TSI-1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,8 +163,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,13 +487,190 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BC42DC-0B2D-4AA2-92F8-4B441B916006}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAC1FA4-43E8-45B7-904F-2DA13FFC07E0}">
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3">
+        <v>3</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0</v>
+      </c>
+      <c r="X2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>7</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>